<commit_message>
Updated Scrum documents and added the Sprint 6 burndown chart and Sprint backlog
</commit_message>
<xml_diff>
--- a/Project/Scrum board.xlsx
+++ b/Project/Scrum board.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dani_\IdeaProjects\jabref\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Filipe\Documents\ES\jabref\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57EE06E1-EAE2-4A05-8A0A-9EC885CDFEC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F075A2E3-1627-4813-84E4-A6A886F30579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{002D318A-516A-4F53-BD99-44FA86C91C20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{002D318A-516A-4F53-BD99-44FA86C91C20}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="65">
   <si>
     <t>Task Number</t>
   </si>
@@ -217,6 +217,18 @@
   </si>
   <si>
     <t>Sprint 1 backlog</t>
+  </si>
+  <si>
+    <t>Sprint 6 backlog</t>
+  </si>
+  <si>
+    <t>Implement Webcam</t>
+  </si>
+  <si>
+    <t>Test Webcam</t>
+  </si>
+  <si>
+    <t>António/Daniel</t>
   </si>
 </sst>
 </file>
@@ -282,13 +294,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -309,7 +324,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -605,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE69595-3AF5-4C07-8250-C145B7C5032F}">
-  <dimension ref="A2:H56"/>
+  <dimension ref="A2:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,6 +1594,90 @@
         <v>10</v>
       </c>
     </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="3">
+        <v>1</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="3">
+        <v>2</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Scrum master week 4 updated.
</commit_message>
<xml_diff>
--- a/Project/Scrum board.xlsx
+++ b/Project/Scrum board.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Filipe\Documents\ES\jabref\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\IdeaProjects\jabref\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F075A2E3-1627-4813-84E4-A6A886F30579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63C1703-6517-4E6C-BCA2-DB9595CCB854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{002D318A-516A-4F53-BD99-44FA86C91C20}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="66">
   <si>
     <t>Task Number</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>António/Daniel</t>
+  </si>
+  <si>
+    <t>Planning/Building use case diagrams</t>
   </si>
 </sst>
 </file>
@@ -258,7 +261,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -290,6 +293,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -303,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -620,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE69595-3AF5-4C07-8250-C145B7C5032F}">
-  <dimension ref="A2:H63"/>
+  <dimension ref="A2:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,87 +1614,116 @@
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="4">
+        <v>1</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="3" t="s">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D63" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E63" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F59" s="3" t="s">
+      <c r="F63" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G59" s="3" t="s">
+      <c r="G63" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H59" s="3" t="s">
+      <c r="H63" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="3">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="3">
         <v>1</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D64" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E64" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="3">
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="3">
         <v>2</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D65" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E65" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F61" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
+      <c r="F65" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated some scrum docs
</commit_message>
<xml_diff>
--- a/Project/Scrum board.xlsx
+++ b/Project/Scrum board.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\IdeaProjects\jabref\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Filipe\Documents\ES\jabref\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63C1703-6517-4E6C-BCA2-DB9595CCB854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF4273B-1DE9-450C-9A49-3ACBAF6A2BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{002D318A-516A-4F53-BD99-44FA86C91C20}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="64">
   <si>
     <t>Task Number</t>
   </si>
@@ -219,13 +219,7 @@
     <t>Sprint 1 backlog</t>
   </si>
   <si>
-    <t>Sprint 6 backlog</t>
-  </si>
-  <si>
     <t>Implement Webcam</t>
-  </si>
-  <si>
-    <t>Test Webcam</t>
   </si>
   <si>
     <t>António/Daniel</t>
@@ -312,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,6 +316,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -640,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE69595-3AF5-4C07-8250-C145B7C5032F}">
   <dimension ref="A2:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,7 +1642,7 @@
         <v>1</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>8</v>
@@ -1661,7 +1658,7 @@
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
@@ -1692,10 +1689,10 @@
         <v>1</v>
       </c>
       <c r="C64" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>9</v>
@@ -1707,23 +1704,13 @@
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="3">
-        <v>2</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>